<commit_message>
add correct data spreadsheet
</commit_message>
<xml_diff>
--- a/Unilever interactive revised VALUES.xlsx
+++ b/Unilever interactive revised VALUES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28680" windowHeight="15800" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="_CIQHiddenCacheSheet" sheetId="12" state="veryHidden" r:id="rId1"/>
-    <sheet name="assumptions and outputs" sheetId="2" r:id="rId2"/>
+    <sheet name="assumptions and outputs" sheetId="2" r:id="rId1"/>
+    <sheet name="_CIQHiddenCacheSheet" sheetId="13" state="veryHidden" r:id="rId2"/>
     <sheet name="Model" sheetId="1" r:id="rId3"/>
     <sheet name="company by company input" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -45,17 +45,12 @@
     <definedName name="IQ_YTD" hidden="1">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="140001" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="136">
   <si>
     <t>Assumptions</t>
   </si>
@@ -372,7 +367,97 @@
     <t>cyMDEuOTU5MjMBDgAAAAUAAAACMTEBAAAAATACAAAACjEwMDMxMTkzOTMDAAAABjEwMDE4MQQAAAABMgYAAAABMAcAAAADMTYwCAAAAAEwCQAAAAExCgAAAAEwCwAAAAsxMDAyNzQzOTYyOQwAAAABNw0AAAAJMi8yOC8yMDE3EAAAAAkyLzI3LzIwMTfwN8wBRF/UCGXd0QFEX9QIJ0NJUS5LSEMuSVFfRUJJVERBX01FRElBTl9FU1RfQ0lRLkNZMjAxOAEAAACojRAPAgAAAAg4OTE0LjgyNQEOAAAABQAAAAIxMQEAAAABMAIAAAAKMTAwMzExOTM5MwMAAAAGMTAwMTg4BAAAAAEyBgAAAAEwBwAAAAMxNjAIAAAAATAJAAAAATEKAAAAATALAAAACzEwMDI3MzI4NzI3DAAAAAE3DQAAAAkyLzI4LzIwMTcQAAAACTIvMjcvMjAxN/A3zAFEX9QIdgTSAURf1AgoQ0lRLktIQy5JUV9SRVZFTlVFX01FRElBTl9FU1RfQ0lRLkNZMjAxOQEAAACojRAPAgAAAAsyNzg4OC4wNDE1MwEOAAAABQAAAAIxMQEAAAABMAIAAAAKMTAwMzExOTM5OAMAAAAGMTAwMTgxBAAAAAEyBgAAAAEwBwAAAAMxNjAIAAAAATAJAAAAATEKAAAAATALAAAACzEwMDI3NDM5OTg5DAAAAAE3DQAAAAkyLzI4LzIwMTcQAAAACTIvMjcvMjAxN/A3zAFEX9QIZd3RAURf1Ag=</t>
   </si>
   <si>
-    <t>`</t>
+    <t>synergies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=(4.11*1230) + (2.46*2840) </t>
+  </si>
+  <si>
+    <t>=( + -.08*((44.97*1.06*(1+.25)*2840)-15000-(2840*(45.26*(1+.25)*.25))+ .25*14400*1.06)* (1-.35))</t>
+  </si>
+  <si>
+    <t>synergies + interest expense (tax affected)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>pro forma shares</t>
+  </si>
+  <si>
+    <t>=1230 +(( 45.26*1.06*(1+.25)*.25)/94.87)) + 15000/94.87</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>(a+ b) / c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>(d - 4.11) / 4.11</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>(Kraft 2017E Earnings * Kraft shares)+ (Target 2017E Earnings + Target Shares)</t>
+  </si>
+  <si>
+    <t>[ cost of debt * (standalone target stock price * target share count * exchange rate)* (1+ premium) * share count)- Berkshire-3G contribution- ( (standalone target stock price * target share count * exchange rate)* (1+ premium) * share count* % stock consideration)] * 1- tax rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pro forma net income                            </t>
+  </si>
+  <si>
+    <t>d/ stanalone 2018E Kraft EPS</t>
+  </si>
+  <si>
+    <t>EPS accretion</t>
+  </si>
+  <si>
+    <t>leverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">= Kraft standalone debt + target standalone net debt + [ (standalone target stock price * target share count * exchange rate)* (1+ premium) * share count)- Berkshire-3G contribution- ( (standalone target stock price * target share count * exchange rate)* (1+ premium) * share count* % stock consideration)] </t>
+  </si>
+  <si>
+    <t>= Kraft 2017E EBITDA + Target 2017E EBITDA</t>
+  </si>
+  <si>
+    <t>a/b</t>
+  </si>
+  <si>
+    <t>Pro forma total debt</t>
+  </si>
+  <si>
+    <t>Pro forma Ebitda</t>
+  </si>
+  <si>
+    <t>Buffett/3G ownership</t>
+  </si>
+  <si>
+    <t>Kraft standalone shares + ((target stock price * exchange rate) * (1+ premium)* % stock)/Kraft stock price + Berkshire_3G contribution/Kraft stock price</t>
+  </si>
+  <si>
+    <t>Berkshire_3G shares issued</t>
+  </si>
+  <si>
+    <t>Berkshire_3G contribution/Kraft stock price</t>
+  </si>
+  <si>
+    <t>existing Berkshire_3G shares</t>
+  </si>
+  <si>
+    <t>a + b + c</t>
   </si>
 </sst>
 </file>
@@ -380,16 +465,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0%_);\(#,##0.0%\)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0\x"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0000\x"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0_);\(#,##0.0\)"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0%_);\(#,##0.0%\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0\x"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000\x"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_);\(#,##0.0\)"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +603,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -533,7 +626,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -545,30 +638,30 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -576,14 +669,14 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,46 +684,46 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -639,7 +732,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -647,17 +740,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -667,7 +760,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -675,12 +768,12 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,18 +782,40 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -708,92 +823,103 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="7" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="5" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="7" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="7" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="37" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="37" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="39" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="5" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +935,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="70" dropStyle="combo" dx="16" fmlaLink="'company by company input'!$G$7" fmlaRange="$S$6:$S$12" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="'company by company input'!$G$7" fmlaRange="$S$6:$S$12" noThreeD="1" sel="7" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,9 +951,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>177800</xdr:colOff>
+          <xdr:colOff>171450</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>238125</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1144,64 +1270,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:S102"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5" style="19" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" style="19" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:19" ht="14">
+    <row r="1" spans="4:19" ht="15" x14ac:dyDescent="0.25">
       <c r="N1"/>
     </row>
-    <row r="2" spans="4:19" ht="14">
+    <row r="2" spans="4:19" ht="15" x14ac:dyDescent="0.25">
       <c r="N2"/>
     </row>
-    <row r="3" spans="4:19" ht="25">
+    <row r="3" spans="4:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="N3" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="4:19" ht="36">
+    <row r="4" spans="4:19" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="D4" s="18" t="s">
         <v>38</v>
       </c>
@@ -1210,8 +1304,8 @@
       </c>
       <c r="O4" s="19"/>
     </row>
-    <row r="5" spans="4:19" ht="20" thickBot="1"/>
-    <row r="6" spans="4:19" ht="20" thickBot="1">
+    <row r="5" spans="4:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="4:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" s="19" t="s">
         <v>82</v>
       </c>
@@ -1224,7 +1318,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="4:19">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E7" s="19" t="s">
         <v>80</v>
       </c>
@@ -1242,7 +1336,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="4:19">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E8" s="19" t="s">
         <v>81</v>
       </c>
@@ -1260,7 +1354,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="4:19">
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E9" s="19" t="s">
         <v>78</v>
       </c>
@@ -1278,12 +1372,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="4:19" ht="20" thickBot="1">
+    <row r="10" spans="4:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E10" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="62">
-        <v>0.3</v>
+      <c r="N10" s="61">
+        <v>0.1</v>
       </c>
       <c r="P10" s="31">
         <v>0</v>
@@ -1296,380 +1390,380 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="4:19" ht="14">
+    <row r="11" spans="4:19" ht="15" x14ac:dyDescent="0.25">
       <c r="N11"/>
       <c r="S11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="4:19">
+    <row r="12" spans="4:19" x14ac:dyDescent="0.3">
       <c r="S12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="4:19" ht="36">
+    <row r="13" spans="4:19" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="4:19" ht="36">
+    <row r="14" spans="4:19" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="4:19">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E15" s="19" t="s">
         <v>64</v>
       </c>
       <c r="N15" s="24">
         <f ca="1">Model!H16/(Model!H16+Model!F16*Model!F28)</f>
-        <v>0.50780294388205416</v>
-      </c>
-    </row>
-    <row r="16" spans="4:19">
+        <v>0.30049584009481817</v>
+      </c>
+    </row>
+    <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E16" s="19" t="str">
         <f ca="1">" % 2017E Revenue from "&amp; Model!$F$5</f>
-        <v xml:space="preserve"> % 2017E Revenue from MDLZ</v>
+        <v xml:space="preserve"> % 2017E Revenue from ENXTAM:UNA</v>
       </c>
       <c r="N16" s="24">
         <f ca="1">1-N15</f>
-        <v>0.49219705611794584</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14">
+        <v>0.69950415990518189</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E17" s="19"/>
       <c r="N17" s="25"/>
     </row>
-    <row r="18" spans="5:14">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E18" s="19" t="s">
         <v>65</v>
       </c>
       <c r="N18" s="24">
         <f ca="1">Model!H20/(Model!H20+Model!F20*Model!F28)</f>
-        <v>0.62190926516296019</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14">
+        <v>0.42261488963544519</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E19" s="19" t="str">
         <f ca="1">" % 2017E EBITDA from "&amp; Model!$F$5</f>
-        <v xml:space="preserve"> % 2017E EBITDA from MDLZ</v>
+        <v xml:space="preserve"> % 2017E EBITDA from ENXTAM:UNA</v>
       </c>
       <c r="N19" s="24">
         <f ca="1">1-N18</f>
-        <v>0.37809073483703981</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14">
+        <v>0.57738511036455487</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E20" s="19"/>
       <c r="N20" s="25"/>
     </row>
-    <row r="21" spans="5:14">
+    <row r="21" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E21" s="19" t="s">
         <v>46</v>
       </c>
       <c r="N21" s="24">
         <f ca="1">Model!G66</f>
-        <v>9.7954346902709863E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="5:14">
+        <v>1.3107100802752663E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E22" s="19"/>
       <c r="N22" s="25"/>
     </row>
-    <row r="23" spans="5:14">
+    <row r="23" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E23" s="19" t="s">
         <v>43</v>
       </c>
       <c r="N23" s="26">
         <f ca="1">Model!O7</f>
-        <v>86815.243248375002</v>
-      </c>
-    </row>
-    <row r="24" spans="5:14">
+        <v>160643.72087473</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E24" s="19" t="s">
         <v>44</v>
       </c>
       <c r="N24" s="26">
         <f ca="1">Model!O10</f>
-        <v>102327.243248375</v>
-      </c>
-    </row>
-    <row r="25" spans="5:14">
+        <v>174678.12087473</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E25" s="19" t="s">
         <v>45</v>
       </c>
       <c r="N25" s="26">
         <f ca="1">Model!T5</f>
-        <v>50111.432436281248</v>
-      </c>
-    </row>
-    <row r="26" spans="5:14">
+        <v>105482.79065604749</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E26" s="19" t="s">
         <v>91</v>
       </c>
       <c r="N26" s="26">
         <f ca="1">Model!T5+Model!F11+Model!H11</f>
-        <v>93769.432436281248</v>
-      </c>
-    </row>
-    <row r="27" spans="5:14">
+        <v>147053.63065604749</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E27" s="19"/>
       <c r="N27" s="25"/>
     </row>
-    <row r="28" spans="5:14">
+    <row r="28" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E28" s="19" t="s">
         <v>41</v>
       </c>
       <c r="N28" s="27">
         <f>Model!O27</f>
-        <v>3.360296983905386</v>
-      </c>
-    </row>
-    <row r="29" spans="5:14">
+        <v>3.3539486203615603</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E29" s="19" t="s">
         <v>42</v>
       </c>
       <c r="N29" s="27">
         <f ca="1">Model!O28</f>
-        <v>6.9489128998600016</v>
-      </c>
-    </row>
-    <row r="30" spans="5:14">
+        <v>7.6411487171134462</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E30" s="19"/>
       <c r="N30" s="25"/>
     </row>
-    <row r="31" spans="5:14">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E31" s="19" t="s">
         <v>37</v>
       </c>
       <c r="N31" s="24">
         <f ca="1">Model!O23</f>
-        <v>0.37960175427132758</v>
-      </c>
-    </row>
-    <row r="32" spans="5:14">
+        <v>0.33883445196936202</v>
+      </c>
+    </row>
+    <row r="32" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E32" s="19" t="str">
         <f ca="1">Model!F5&amp;" ownership"</f>
-        <v>MDLZ ownership</v>
+        <v>ENXTAM:UNA ownership</v>
       </c>
       <c r="N32" s="24">
         <f ca="1">Model!O24</f>
-        <v>0.14148046710992029</v>
-      </c>
-    </row>
-    <row r="33" spans="5:14">
+        <v>0.23368110879730192</v>
+      </c>
+    </row>
+    <row r="33" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E33" s="19" t="s">
         <v>92</v>
       </c>
       <c r="N33" s="24">
         <f ca="1">Model!O25</f>
-        <v>0.47891777861875212</v>
-      </c>
-    </row>
-    <row r="34" spans="5:14">
+        <v>0.42748443923333607</v>
+      </c>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E34" s="19"/>
       <c r="N34" s="24"/>
     </row>
-    <row r="35" spans="5:14">
+    <row r="35" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E35" s="19"/>
     </row>
-    <row r="36" spans="5:14">
+    <row r="36" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E36" s="19"/>
     </row>
-    <row r="37" spans="5:14">
+    <row r="37" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E37" s="19"/>
     </row>
-    <row r="38" spans="5:14">
+    <row r="38" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="5:14">
+    <row r="39" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E39" s="19"/>
     </row>
-    <row r="40" spans="5:14">
+    <row r="40" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="5:14">
+    <row r="41" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E41" s="19"/>
     </row>
-    <row r="42" spans="5:14">
+    <row r="42" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E42" s="19"/>
     </row>
-    <row r="43" spans="5:14">
+    <row r="43" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E43" s="19"/>
     </row>
-    <row r="44" spans="5:14">
+    <row r="44" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E44" s="19"/>
     </row>
-    <row r="45" spans="5:14">
+    <row r="45" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E45" s="19"/>
     </row>
-    <row r="46" spans="5:14">
+    <row r="46" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E46" s="19"/>
     </row>
-    <row r="47" spans="5:14">
+    <row r="47" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E47" s="19"/>
     </row>
-    <row r="48" spans="5:14">
+    <row r="48" spans="5:14" x14ac:dyDescent="0.3">
       <c r="E48" s="19"/>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="19"/>
     </row>
-    <row r="50" spans="5:5">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="19"/>
     </row>
-    <row r="51" spans="5:5">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="19"/>
     </row>
-    <row r="52" spans="5:5">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="19"/>
     </row>
-    <row r="53" spans="5:5">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="19"/>
     </row>
-    <row r="54" spans="5:5">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="19"/>
     </row>
-    <row r="55" spans="5:5">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="19"/>
     </row>
-    <row r="56" spans="5:5">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="19"/>
     </row>
-    <row r="57" spans="5:5">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="19"/>
     </row>
-    <row r="58" spans="5:5">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="19"/>
     </row>
-    <row r="59" spans="5:5">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="19"/>
     </row>
-    <row r="60" spans="5:5">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="19"/>
     </row>
-    <row r="61" spans="5:5">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="19"/>
     </row>
-    <row r="62" spans="5:5">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="19"/>
     </row>
-    <row r="63" spans="5:5">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="19"/>
     </row>
-    <row r="64" spans="5:5">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="19"/>
     </row>
-    <row r="65" spans="5:5">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="19"/>
     </row>
-    <row r="66" spans="5:5">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="19"/>
     </row>
-    <row r="67" spans="5:5">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="19"/>
     </row>
-    <row r="68" spans="5:5">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="19"/>
     </row>
-    <row r="69" spans="5:5">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="19"/>
     </row>
-    <row r="70" spans="5:5">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="19"/>
     </row>
-    <row r="71" spans="5:5">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="19"/>
     </row>
-    <row r="72" spans="5:5">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="19"/>
     </row>
-    <row r="73" spans="5:5">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="19"/>
     </row>
-    <row r="74" spans="5:5">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="19"/>
     </row>
-    <row r="75" spans="5:5">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="19"/>
     </row>
-    <row r="76" spans="5:5">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="19"/>
     </row>
-    <row r="77" spans="5:5">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="19"/>
     </row>
-    <row r="78" spans="5:5">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="19"/>
     </row>
-    <row r="79" spans="5:5">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="19"/>
     </row>
-    <row r="80" spans="5:5">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="5:5">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="19"/>
     </row>
-    <row r="82" spans="5:5">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="19"/>
     </row>
-    <row r="83" spans="5:5">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="19"/>
     </row>
-    <row r="84" spans="5:5">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="19"/>
     </row>
-    <row r="85" spans="5:5">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="19"/>
     </row>
-    <row r="86" spans="5:5">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="19"/>
     </row>
-    <row r="87" spans="5:5">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E87" s="19"/>
     </row>
-    <row r="88" spans="5:5">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E88" s="19"/>
     </row>
-    <row r="89" spans="5:5">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E89" s="19"/>
     </row>
-    <row r="90" spans="5:5">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E90" s="19"/>
     </row>
-    <row r="91" spans="5:5">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E91" s="19"/>
     </row>
-    <row r="92" spans="5:5">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E92" s="19"/>
     </row>
-    <row r="93" spans="5:5">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E93" s="19"/>
     </row>
-    <row r="94" spans="5:5">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E94" s="19"/>
     </row>
-    <row r="95" spans="5:5">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E95" s="19"/>
     </row>
-    <row r="96" spans="5:5">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E96" s="19"/>
     </row>
-    <row r="97" spans="5:5">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E97" s="19"/>
     </row>
-    <row r="98" spans="5:5">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E98" s="19"/>
     </row>
-    <row r="99" spans="5:5">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E99" s="19"/>
     </row>
-    <row r="100" spans="5:5">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E100" s="19"/>
     </row>
-    <row r="101" spans="5:5">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E101" s="19"/>
     </row>
-    <row r="102" spans="5:5">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E102" s="19"/>
     </row>
   </sheetData>
@@ -1695,15 +1789,15 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId3" name="Drop Down 6">
+            <control shapeId="2054" r:id="rId4" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -1714,53 +1808,73 @@
                   </from>
                   <to>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>177800</xdr:colOff>
+                    <xdr:colOff>171450</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>238125</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y66"/>
+  <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D42" workbookViewId="0">
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1775,10 +1889,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="str">
         <f ca="1">OFFSET('company by company input'!M5,0,'company by company input'!G7)</f>
-        <v>MDLZ</v>
+        <v>ENXTAM:UNA</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>73</v>
@@ -1791,24 +1905,24 @@
       <c r="N5" s="38"/>
       <c r="O5" s="40">
         <f ca="1">F7*(1+'assumptions and outputs'!N7)</f>
-        <v>56.212499999999999</v>
+        <v>56.570875000000001</v>
       </c>
       <c r="Q5" t="s">
         <v>17</v>
       </c>
       <c r="T5" s="3">
         <f ca="1">Y8-SUM(T6:T7)</f>
-        <v>50111.432436281248</v>
+        <v>105482.79065604749</v>
       </c>
       <c r="W5" t="s">
         <v>16</v>
       </c>
       <c r="Y5" s="42">
         <f ca="1">O7</f>
-        <v>86815.243248375002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+        <v>160643.72087473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F6" s="8"/>
       <c r="H6" s="8"/>
       <c r="K6" s="38" t="s">
@@ -1819,7 +1933,7 @@
       <c r="N6" s="38"/>
       <c r="O6" s="39">
         <f ca="1">F8</f>
-        <v>1544.4117100000001</v>
+        <v>2839.6895199999999</v>
       </c>
       <c r="Q6" t="s">
         <v>85</v>
@@ -1830,13 +1944,13 @@
       </c>
       <c r="Y6" s="28"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="46">
         <f ca="1">OFFSET('company by company input'!M7,0,'company by company input'!G7)*F28</f>
-        <v>44.97</v>
+        <v>45.256700000000002</v>
       </c>
       <c r="H7" s="46">
         <f>'company by company input'!V7</f>
@@ -1851,24 +1965,24 @@
       <c r="N7" s="8"/>
       <c r="O7" s="15">
         <f ca="1">O5*O6</f>
-        <v>86815.243248375002</v>
+        <v>160643.72087473</v>
       </c>
       <c r="Q7" t="str">
         <f ca="1">"Value of shares issued to " &amp;Model!F5</f>
-        <v>Value of shares issued to MDLZ</v>
+        <v>Value of shares issued to ENXTAM:UNA</v>
       </c>
       <c r="T7" s="34">
         <f ca="1">O20</f>
-        <v>21703.81081209375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+        <v>40160.930218682501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="41">
         <f ca="1">OFFSET('company by company input'!M8,0,'company by company input'!G7)</f>
-        <v>1544.4117100000001</v>
+        <v>2839.6895199999999</v>
       </c>
       <c r="H8" s="41">
         <f>'company by company input'!V8</f>
@@ -1879,23 +1993,23 @@
       </c>
       <c r="T8" s="15">
         <f ca="1">SUM(T5:T7)</f>
-        <v>86815.243248375002</v>
+        <v>160643.72087473</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="Y8" s="15">
         <f ca="1">SUM(Y5:Y7)</f>
-        <v>86815.243248375002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
+        <v>160643.72087473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F9" s="15">
         <f ca="1">F7*F8</f>
-        <v>69452.194598700007</v>
+        <v>128514.97669978401</v>
       </c>
       <c r="H9" s="15">
         <f>H7*H8</f>
@@ -1903,24 +2017,24 @@
       </c>
       <c r="O9" s="34"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>54</v>
       </c>
       <c r="O10" s="3">
         <f ca="1">O7+F11+F12</f>
-        <v>102327.243248375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+        <v>174678.12087473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F11" s="47">
         <f ca="1">OFFSET('company by company input'!M10,0,'company by company input'!$G$7)*Model!$F$28</f>
-        <v>15458</v>
-      </c>
-      <c r="H11" s="55">
+        <v>13370.84</v>
+      </c>
+      <c r="H11" s="54">
         <f>'company by company input'!V10</f>
         <v>28200</v>
       </c>
@@ -1929,18 +2043,18 @@
       </c>
       <c r="O11" s="6">
         <f ca="1">O10/F20</f>
-        <v>20.056300127082515</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+        <v>16.118732485084795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F12" s="47">
         <f ca="1">OFFSET('company by company input'!M11,0,'company by company input'!$G$7)*Model!$F$28</f>
-        <v>54</v>
-      </c>
-      <c r="H12" s="54">
+        <v>663.56000000000006</v>
+      </c>
+      <c r="H12" s="53">
         <f>'company by company input'!T11</f>
         <v>626</v>
       </c>
@@ -1950,10 +2064,10 @@
       </c>
       <c r="O12" s="6">
         <f ca="1">O5/F24</f>
-        <v>26.767857142857142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25">
+        <v>26.551616915422887</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1961,7 +2075,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="16">
         <f ca="1">F9+F11+F12</f>
-        <v>84964.194598700007</v>
+        <v>142549.37669978401</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="16"/>
@@ -1970,65 +2084,62 @@
       </c>
       <c r="O14" s="4">
         <f ca="1">O5-O15</f>
-        <v>42.159374999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
+        <v>42.428156250000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>12</v>
       </c>
       <c r="O15" s="4">
         <f ca="1">O5*'assumptions and outputs'!N8</f>
-        <v>14.053125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+        <v>14.14271875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="47">
         <f ca="1">OFFSET('company by company input'!M17,0,'company by company input'!$G$7)*$F$28</f>
-        <v>25852.31149</v>
+        <v>58602.100000000006</v>
       </c>
       <c r="H16" s="30">
-        <f>'company by company input'!Y2+'company by company input'!V17</f>
-        <v>26672</v>
+        <v>26685</v>
       </c>
       <c r="K16" t="s">
         <v>58</v>
       </c>
       <c r="O16" s="9">
         <f ca="1">O15/H7</f>
-        <v>0.1481303362496047</v>
-      </c>
-    </row>
-    <row r="17" spans="3:16">
+        <v>0.14907472067039107</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="47">
         <f ca="1">OFFSET('company by company input'!M18,0,'company by company input'!$G$7)*$F$28</f>
-        <v>26420.626960000001</v>
+        <v>60934.529830000007</v>
       </c>
       <c r="H17" s="28">
-        <f>'company by company input'!V18</f>
-        <v>27201.95923</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16">
+        <v>27181</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="47">
         <f ca="1">OFFSET('company by company input'!M19,0,'company by company input'!$G$7)*$F$28</f>
-        <v>27199.109840000001</v>
+        <v>63912.680538400004</v>
       </c>
       <c r="H18" s="28">
-        <f>'company by company input'!V19</f>
-        <v>27888.041529999999</v>
-      </c>
-    </row>
-    <row r="19" spans="3:16">
+        <v>27746</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F19" s="41"/>
       <c r="H19" s="7"/>
       <c r="K19" t="s">
@@ -2036,40 +2147,38 @@
       </c>
       <c r="O19" s="3">
         <f ca="1">O14*O6</f>
-        <v>65111.432436281248</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16">
+        <v>120482.79065604749</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="47">
         <f ca="1">OFFSET('company by company input'!M21,0,'company by company input'!$G$7)*$F$28</f>
-        <v>5102</v>
+        <v>10836.9638268</v>
       </c>
       <c r="H20" s="30">
-        <f>'company by company input'!V21</f>
-        <v>8392.1153799999993</v>
+        <v>8408</v>
       </c>
       <c r="K20" t="s">
         <v>60</v>
       </c>
       <c r="O20" s="4">
         <f ca="1">O15*O6</f>
-        <v>21703.81081209375</v>
-      </c>
-    </row>
-    <row r="21" spans="3:16">
+        <v>40160.930218682501</v>
+      </c>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="47">
         <f ca="1">OFFSET('company by company input'!M22,0,'company by company input'!$G$7)*$F$28</f>
-        <v>5479.9736800000001</v>
+        <v>11620.78</v>
       </c>
       <c r="H21" s="28">
-        <f>'company by company input'!V22</f>
-        <v>8914.8250000000007</v>
+        <v>8956</v>
       </c>
       <c r="K21" s="11" t="s">
         <v>31</v>
@@ -2081,115 +2190,111 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:16">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="47">
         <f ca="1">OFFSET('company by company input'!M23,0,'company by company input'!$G$7)*$F$28</f>
-        <v>5791</v>
+        <v>12473.02</v>
       </c>
       <c r="H22" s="28">
-        <f>'company by company input'!V23</f>
-        <v>9259</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16">
+        <v>9209</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
         <v>37</v>
       </c>
       <c r="O23" s="5">
         <f ca="1">1-SUM(O24:O26)</f>
-        <v>0.37960175427132758</v>
-      </c>
-    </row>
-    <row r="24" spans="3:16">
+        <v>0.33883445196936202</v>
+      </c>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="46">
         <f ca="1">OFFSET('company by company input'!M25,0,'company by company input'!$G$7)*$F$28</f>
-        <v>2.1</v>
+        <v>2.1305999999999998</v>
       </c>
       <c r="H24" s="29">
-        <f>'company by company input'!V25</f>
-        <v>3.76</v>
+        <v>3.77</v>
       </c>
       <c r="K24" t="str">
         <f ca="1">Model!F5&amp;" ownership"</f>
-        <v>MDLZ ownership</v>
+        <v>ENXTAM:UNA ownership</v>
       </c>
       <c r="O24" s="5">
         <f ca="1">G57/$G$59</f>
-        <v>0.14148046710992029</v>
-      </c>
-    </row>
-    <row r="25" spans="3:16">
+        <v>0.23368110879730192</v>
+      </c>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="46">
         <f ca="1">OFFSET('company by company input'!M26,0,'company by company input'!$G$7)*$F$28</f>
-        <v>2.3312499999999998</v>
+        <v>2.318962</v>
       </c>
       <c r="H25" s="32">
-        <f>'company by company input'!V26</f>
-        <v>4.16</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="K25" t="s">
         <v>84</v>
       </c>
       <c r="O25" s="5">
         <f ca="1">(P25+P26+G58)/G59</f>
-        <v>0.47891777861875212</v>
+        <v>0.42748443923333607</v>
       </c>
       <c r="P25">
         <v>325.60000000000002</v>
       </c>
     </row>
-    <row r="26" spans="3:16">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="46">
         <f ca="1">OFFSET('company by company input'!M27,0,'company by company input'!$G$7)*$F$28</f>
-        <v>2.5499100000000001</v>
+        <v>2.5228000000000002</v>
       </c>
       <c r="H26" s="32">
-        <f>'company by company input'!V27</f>
-        <v>4.36693</v>
+        <v>4.33</v>
       </c>
       <c r="O26" s="5"/>
       <c r="P26">
         <v>290.7</v>
       </c>
     </row>
-    <row r="27" spans="3:16">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
         <v>83</v>
       </c>
       <c r="O27" s="6">
         <f>H11/H20</f>
-        <v>3.360296983905386</v>
-      </c>
-    </row>
-    <row r="28" spans="3:16">
+        <v>3.3539486203615603</v>
+      </c>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="48">
         <f ca="1">OFFSET('company by company input'!M32,0,'company by company input'!G7)</f>
-        <v>1</v>
+        <v>1.06</v>
       </c>
       <c r="K28" t="s">
         <v>90</v>
       </c>
       <c r="O28" s="6">
         <f ca="1">(F11+H11+T5)/(F20+H20)</f>
-        <v>6.9489128998600016</v>
-      </c>
-    </row>
-    <row r="29" spans="3:16">
+        <v>7.6411487171134462</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>34</v>
       </c>
@@ -2197,7 +2302,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="30" spans="3:16">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>35</v>
       </c>
@@ -2205,7 +2310,16 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="33" spans="3:10">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="41">
+        <f ca="1">OFFSET('company by company input'!M29,0,'company by company input'!G7)*F28*'assumptions and outputs'!N10</f>
+        <v>1526.4</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="G33" s="1">
         <v>2018</v>
       </c>
@@ -2214,7 +2328,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
@@ -2224,20 +2338,31 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="3:10">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="J35" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>51</v>
       </c>
       <c r="G36" s="33">
         <f>H25</f>
-        <v>4.16</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="H36" s="33">
         <f>H26</f>
-        <v>4.36693</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10">
+        <v>4.33</v>
+      </c>
+      <c r="J36" t="s">
+        <v>109</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>1</v>
       </c>
@@ -2249,147 +2374,213 @@
         <f>G37</f>
         <v>1230.1168700000001</v>
       </c>
-    </row>
-    <row r="38" spans="3:10">
+      <c r="K37" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
       <c r="G38" s="14">
         <f>G36*G37</f>
-        <v>5117.2861792000003</v>
+        <v>5055.7803357000003</v>
       </c>
       <c r="H38" s="14">
         <f>H36*H37</f>
-        <v>5371.8342631091</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10">
+        <v>5326.4060471000003</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>110</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f ca="1">F5&amp;" EPS Estimate ($)"</f>
-        <v>MDLZ EPS Estimate ($)</v>
+        <v>ENXTAM:UNA EPS Estimate ($)</v>
       </c>
       <c r="G40" s="33">
         <f ca="1">F25*F28</f>
-        <v>2.3312499999999998</v>
+        <v>2.4580997199999999</v>
       </c>
       <c r="H40" s="33">
         <f ca="1">F26*F28</f>
-        <v>2.5499100000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10">
+        <v>2.6741680000000003</v>
+      </c>
+      <c r="K40" s="74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="G41" s="34">
         <f ca="1">F8</f>
-        <v>1544.4117100000001</v>
+        <v>2839.6895199999999</v>
       </c>
       <c r="H41" s="34">
         <f ca="1">G41</f>
-        <v>1544.4117100000001</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10">
+        <v>2839.6895199999999</v>
+      </c>
+    </row>
+    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>61</v>
       </c>
       <c r="G42" s="14">
         <f ca="1">G40*G41</f>
-        <v>3600.4097989375</v>
+        <v>6980.240013998934</v>
       </c>
       <c r="H42" s="14">
         <f ca="1">H40*H41</f>
-        <v>3938.1108634461002</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10">
+        <v>7593.8068443193606</v>
+      </c>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G44" s="16">
         <f ca="1">G38+G42</f>
-        <v>8717.6959781375008</v>
+        <v>12036.020349698934</v>
       </c>
       <c r="H44" s="16">
         <f ca="1">H38+H42</f>
-        <v>9309.9451265551997</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10">
+        <v>12920.21289141936</v>
+      </c>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="K45" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="3:10">
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>20</v>
       </c>
       <c r="G47" s="3">
         <f ca="1">-F29*T5</f>
-        <v>-4008.9145949025001</v>
+        <v>-8438.6232524837997</v>
       </c>
       <c r="H47" s="3">
         <f ca="1">G47</f>
-        <v>-4008.9145949025001</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10">
+        <v>-8438.6232524837997</v>
+      </c>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>21</v>
       </c>
-      <c r="F48" t="s">
-        <v>105</v>
-      </c>
       <c r="G48" s="7">
-        <f ca="1">OFFSET('company by company input'!M29,0,'company by company input'!G7)*F28*'assumptions and outputs'!N10</f>
-        <v>1959.6</v>
+        <f ca="1">F31</f>
+        <v>1526.4</v>
       </c>
       <c r="H48" s="7">
-        <f ca="1">G48</f>
-        <v>1959.6</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8">
+        <f ca="1">F31</f>
+        <v>1526.4</v>
+      </c>
+      <c r="J48" t="s">
+        <v>114</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>22</v>
       </c>
       <c r="G49" s="17">
         <f ca="1">SUM(G47:G48)</f>
-        <v>-2049.3145949025002</v>
+        <v>-6912.2232524838</v>
       </c>
       <c r="H49" s="17">
         <f ca="1">SUM(H47:H48)</f>
-        <v>-2049.3145949025002</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8">
+        <v>-6912.2232524838</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>116</v>
+      </c>
+      <c r="K50" t="s">
+        <v>117</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>23</v>
       </c>
       <c r="G51" s="7">
         <f ca="1">G49*(1-$F$30)</f>
-        <v>-1332.0544866866251</v>
+        <v>-4492.94511411447</v>
       </c>
       <c r="H51" s="7">
         <f ca="1">H49*(1-$F$30)</f>
-        <v>-1332.0544866866251</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8">
+        <v>-4492.94511411447</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J53" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G54" s="16">
         <f ca="1">G44+G51</f>
-        <v>7385.6414914508759</v>
+        <v>7543.0752355844643</v>
       </c>
       <c r="H54" s="16">
         <f ca="1">H44+H51</f>
-        <v>7977.8906398685749</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8">
+        <v>8427.267777304889</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>109</v>
+      </c>
+      <c r="K55" s="81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>25</v>
       </c>
@@ -2402,21 +2593,24 @@
         <v>1230.1168700000001</v>
       </c>
     </row>
-    <row r="57" spans="3:8">
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" t="str">
         <f ca="1">"Shares issued to "&amp; F5</f>
-        <v>Shares issued to MDLZ</v>
+        <v>Shares issued to ENXTAM:UNA</v>
       </c>
       <c r="G57" s="7">
         <f ca="1">O20/H7</f>
-        <v>228.774225910127</v>
+        <v>423.32592198463686</v>
       </c>
       <c r="H57" s="7">
         <f ca="1">G57</f>
-        <v>228.774225910127</v>
-      </c>
-    </row>
-    <row r="58" spans="3:8">
+        <v>423.32592198463686</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>89</v>
       </c>
@@ -2429,104 +2623,162 @@
         <v>158.11109939917782</v>
       </c>
     </row>
-    <row r="59" spans="3:8">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>26</v>
       </c>
       <c r="G59" s="17">
         <f ca="1">SUM(G56:G58)</f>
-        <v>1617.0021953093049</v>
+        <v>1811.5538913838147</v>
       </c>
       <c r="H59" s="17">
         <f ca="1">SUM(H56:H58)</f>
-        <v>1617.0021953093049</v>
-      </c>
-    </row>
-    <row r="62" spans="3:8">
+        <v>1811.5538913838147</v>
+      </c>
+      <c r="J59" t="s">
+        <v>110</v>
+      </c>
+      <c r="K59" s="81" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>111</v>
+      </c>
+      <c r="K61" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>62</v>
       </c>
       <c r="G62" s="4">
         <f ca="1">G54/G59</f>
-        <v>4.5674900831152732</v>
+        <v>4.1638701842993138</v>
       </c>
       <c r="H62" s="4">
         <f ca="1">H54/H59</f>
-        <v>4.9337537469097503</v>
-      </c>
-    </row>
-    <row r="63" spans="3:8">
+        <v>4.6519553281782002</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>63</v>
       </c>
       <c r="G63" s="4">
         <f>G36</f>
-        <v>4.16</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="H63" s="4">
         <f>H36</f>
-        <v>4.36693</v>
-      </c>
-    </row>
-    <row r="65" spans="3:8">
+        <v>4.33</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G65" s="35">
         <f ca="1">G62-G63</f>
-        <v>0.40749008311527302</v>
+        <v>5.3870184299313451E-2</v>
       </c>
       <c r="H65" s="35">
         <f ca="1">H62-H63</f>
-        <v>0.56682374690975035</v>
-      </c>
-    </row>
-    <row r="66" spans="3:8">
+        <v>0.32195532817820016</v>
+      </c>
+      <c r="K65" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G66" s="36">
         <f ca="1">G65/G63</f>
-        <v>9.7954346902709863E-2</v>
+        <v>1.3107100802752663E-2</v>
       </c>
       <c r="H66" s="36">
         <f ca="1">H65/H63</f>
-        <v>0.12979913735959825</v>
+        <v>7.4354579255935374E-2</v>
+      </c>
+      <c r="J66" t="s">
+        <v>109</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>110</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>111</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K74" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F4:V36"/>
+  <dimension ref="F3:V36"/>
   <sheetViews>
-    <sheetView showFormulas="1" showGridLines="0" tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView showGridLines="0" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="6:22">
+    <row r="3" spans="6:22" ht="21" x14ac:dyDescent="0.35">
+      <c r="N3" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="75"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+    </row>
+    <row r="4" spans="6:22" x14ac:dyDescent="0.25">
       <c r="G4" s="43">
         <v>42787</v>
       </c>
@@ -2558,64 +2810,66 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="6:22">
-      <c r="N5" t="s">
+    <row r="5" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="N5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="T5" t="s">
+      <c r="T5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V5" t="s">
+      <c r="U5" s="80"/>
+      <c r="V5" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="6:22">
-      <c r="N6" t="s">
+    <row r="6" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="Q6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="V6" t="s">
+      <c r="U6" s="80"/>
+      <c r="V6" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="6:22">
+    <row r="7" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="52">
-        <v>1</v>
+      <c r="G7" s="51">
+        <v>7</v>
       </c>
       <c r="I7" t="s">
         <v>49</v>
@@ -2641,11 +2895,12 @@
       <c r="T7">
         <v>42.695</v>
       </c>
+      <c r="U7" s="77"/>
       <c r="V7">
         <v>94.87</v>
       </c>
     </row>
-    <row r="8" spans="6:22">
+    <row r="8" spans="6:22" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
         <v>66</v>
       </c>
@@ -2670,11 +2925,15 @@
       <c r="T8" s="44">
         <v>2839.6895199999999</v>
       </c>
+      <c r="U8" s="77"/>
       <c r="V8" s="44">
         <v>1230.1168700000001</v>
       </c>
     </row>
-    <row r="10" spans="6:22">
+    <row r="9" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U9" s="77"/>
+    </row>
+    <row r="10" spans="6:22" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
         <v>76</v>
       </c>
@@ -2699,11 +2958,12 @@
       <c r="T10">
         <v>12614</v>
       </c>
+      <c r="U10" s="77"/>
       <c r="V10">
         <v>28200</v>
       </c>
     </row>
-    <row r="11" spans="6:22">
+    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
         <v>77</v>
       </c>
@@ -2728,54 +2988,66 @@
       <c r="T11">
         <v>626</v>
       </c>
+      <c r="U11" s="77"/>
       <c r="V11">
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="6:22" ht="15" thickBot="1"/>
-    <row r="14" spans="6:22" ht="15" thickBot="1">
-      <c r="I14" s="56" t="s">
+    <row r="12" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U12" s="77"/>
+    </row>
+    <row r="13" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U13" s="77"/>
+    </row>
+    <row r="14" spans="6:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="58">
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="57">
         <f>N8*N7+N10+N11</f>
         <v>84964.194598700007</v>
       </c>
-      <c r="O14" s="58">
+      <c r="O14" s="57">
         <f t="shared" ref="O14:T14" si="1">O8*O7+O10+O11</f>
         <v>33938.235302999994</v>
       </c>
-      <c r="P14" s="58">
+      <c r="P14" s="57">
         <f t="shared" si="1"/>
         <v>70451.501468000002</v>
       </c>
-      <c r="Q14" s="58">
+      <c r="Q14" s="57">
         <f t="shared" si="1"/>
         <v>55122.278345599996</v>
       </c>
-      <c r="R14" s="58">
+      <c r="R14" s="57">
         <f t="shared" si="1"/>
         <v>19851.681569599998</v>
       </c>
-      <c r="S14" s="58">
+      <c r="S14" s="57">
         <f t="shared" si="1"/>
         <v>21277.157837499999</v>
       </c>
-      <c r="T14" s="58">
+      <c r="T14" s="57">
         <f t="shared" si="1"/>
         <v>134480.54405640002</v>
       </c>
-      <c r="U14" s="57"/>
-      <c r="V14" s="59">
+      <c r="U14" s="78"/>
+      <c r="V14" s="58">
         <f t="shared" ref="V14" si="2">V8*V7+V10</f>
         <v>144901.18745690002</v>
       </c>
     </row>
-    <row r="17" spans="9:22">
+    <row r="15" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U15" s="77"/>
+    </row>
+    <row r="16" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="U16" s="77"/>
+    </row>
+    <row r="17" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>2</v>
       </c>
@@ -2800,11 +3072,12 @@
       <c r="T17" s="7">
         <v>55285</v>
       </c>
+      <c r="U17" s="77"/>
       <c r="V17" s="7">
         <v>26672</v>
       </c>
     </row>
-    <row r="18" spans="9:22">
+    <row r="18" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>3</v>
       </c>
@@ -2829,11 +3102,12 @@
       <c r="T18" s="7">
         <v>57485.405500000001</v>
       </c>
+      <c r="U18" s="77"/>
       <c r="V18" s="7">
         <v>27201.95923</v>
       </c>
     </row>
-    <row r="19" spans="9:22">
+    <row r="19" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>4</v>
       </c>
@@ -2858,11 +3132,12 @@
       <c r="T19" s="7">
         <v>60294.981639999998</v>
       </c>
+      <c r="U19" s="77"/>
       <c r="V19" s="7">
         <v>27888.041529999999</v>
       </c>
     </row>
-    <row r="20" spans="9:22">
+    <row r="20" spans="9:22" x14ac:dyDescent="0.25">
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -2870,9 +3145,10 @@
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
+      <c r="U20" s="77"/>
       <c r="V20" s="7"/>
     </row>
-    <row r="21" spans="9:22">
+    <row r="21" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>5</v>
       </c>
@@ -2897,11 +3173,12 @@
       <c r="T21" s="7">
         <v>10223.55078</v>
       </c>
+      <c r="U21" s="77"/>
       <c r="V21" s="7">
         <v>8392.1153799999993</v>
       </c>
     </row>
-    <row r="22" spans="9:22">
+    <row r="22" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>6</v>
       </c>
@@ -2926,11 +3203,12 @@
       <c r="T22" s="7">
         <v>10963</v>
       </c>
+      <c r="U22" s="77"/>
       <c r="V22" s="7">
         <v>8914.8250000000007</v>
       </c>
     </row>
-    <row r="23" spans="9:22">
+    <row r="23" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>8</v>
       </c>
@@ -2955,11 +3233,15 @@
       <c r="T23" s="7">
         <v>11767</v>
       </c>
+      <c r="U23" s="77"/>
       <c r="V23" s="7">
         <v>9259</v>
       </c>
     </row>
-    <row r="25" spans="9:22">
+    <row r="24" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="U24" s="77"/>
+    </row>
+    <row r="25" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
         <v>9</v>
       </c>
@@ -2984,11 +3266,12 @@
       <c r="T25" s="45">
         <v>2.0099999999999998</v>
       </c>
+      <c r="U25" s="77"/>
       <c r="V25" s="45">
         <v>3.76</v>
       </c>
     </row>
-    <row r="26" spans="9:22">
+    <row r="26" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
         <v>10</v>
       </c>
@@ -3013,11 +3296,12 @@
       <c r="T26" s="45">
         <v>2.1877</v>
       </c>
+      <c r="U26" s="77"/>
       <c r="V26" s="45">
         <v>4.16</v>
       </c>
     </row>
-    <row r="27" spans="9:22">
+    <row r="27" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>7</v>
       </c>
@@ -3042,11 +3326,15 @@
       <c r="T27" s="45">
         <v>2.38</v>
       </c>
+      <c r="U27" s="77"/>
       <c r="V27" s="45">
         <v>4.36693</v>
       </c>
     </row>
-    <row r="29" spans="9:22">
+    <row r="28" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="U28" s="77"/>
+    </row>
+    <row r="29" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
         <v>86</v>
       </c>
@@ -3071,172 +3359,178 @@
       <c r="T29" s="7">
         <v>14400</v>
       </c>
+      <c r="U29" s="77"/>
       <c r="V29" s="7"/>
     </row>
-    <row r="32" spans="9:22">
+    <row r="30" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="U30" s="77"/>
+    </row>
+    <row r="31" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="U31" s="77"/>
+    </row>
+    <row r="32" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N32" s="53">
+      <c r="N32" s="52">
         <v>1</v>
       </c>
-      <c r="O32" s="53">
+      <c r="O32" s="52">
         <f>N32</f>
         <v>1</v>
       </c>
-      <c r="P32" s="53">
+      <c r="P32" s="52">
         <f t="shared" ref="P32:S32" si="3">O32</f>
         <v>1</v>
       </c>
-      <c r="Q32" s="53">
+      <c r="Q32" s="52">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R32" s="53">
+      <c r="R32" s="52">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="S32" s="53">
+      <c r="S32" s="52">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="T32" s="53">
+      <c r="T32" s="52">
         <v>1.06</v>
       </c>
-      <c r="U32" s="51"/>
-      <c r="V32" s="53"/>
-    </row>
-    <row r="33" spans="9:22" ht="15" thickBot="1"/>
-    <row r="34" spans="9:22">
-      <c r="I34" s="63" t="s">
+      <c r="U32" s="79"/>
+      <c r="V32" s="52"/>
+    </row>
+    <row r="33" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U33" s="77"/>
+    </row>
+    <row r="34" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I34" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="65">
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="64">
         <f>RATE(2,0,-N17,N19)</f>
         <v>2.5717240794771026E-2</v>
       </c>
-      <c r="O34" s="65">
+      <c r="O34" s="64">
         <f t="shared" ref="O34:T34" si="4">RATE(2,0,-O17,O19)</f>
         <v>3.4816510471291588E-3</v>
       </c>
-      <c r="P34" s="65">
+      <c r="P34" s="64">
         <f t="shared" si="4"/>
         <v>4.2331535734487093E-2</v>
       </c>
-      <c r="Q34" s="65">
+      <c r="Q34" s="64">
         <f t="shared" si="4"/>
         <v>3.514835585703649E-2</v>
       </c>
-      <c r="R34" s="65">
+      <c r="R34" s="64">
         <f t="shared" si="4"/>
         <v>3.3740081792809767E-2</v>
       </c>
-      <c r="S34" s="65">
+      <c r="S34" s="64">
         <f t="shared" si="4"/>
         <v>8.4398397484719105E-3</v>
       </c>
-      <c r="T34" s="66">
+      <c r="T34" s="65">
         <f t="shared" si="4"/>
         <v>4.4328010617637026E-2</v>
       </c>
-      <c r="V34" s="60">
+      <c r="U34" s="77"/>
+      <c r="V34" s="59">
         <f t="shared" ref="V34" si="5">RATE(2,0,-V17,V19)</f>
         <v>2.2542145286551154E-2</v>
       </c>
     </row>
-    <row r="35" spans="9:22">
-      <c r="I35" s="67" t="s">
+    <row r="35" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I35" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="J35" s="68"/>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="68"/>
-      <c r="N35" s="69">
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="68">
         <f>N21/N17</f>
         <v>0.19735179200411221</v>
       </c>
-      <c r="O35" s="69">
+      <c r="O35" s="68">
         <f t="shared" ref="O35:T35" si="6">O21/O17</f>
         <v>0.20763519014006795</v>
       </c>
-      <c r="P35" s="69">
+      <c r="P35" s="68">
         <f t="shared" si="6"/>
         <v>0.29205456426170157</v>
       </c>
-      <c r="Q35" s="69">
+      <c r="Q35" s="68">
         <f t="shared" si="6"/>
         <v>0.22960752908405702</v>
       </c>
-      <c r="R35" s="69">
+      <c r="R35" s="68">
         <f t="shared" si="6"/>
         <v>0.21929408659793814</v>
       </c>
-      <c r="S35" s="69">
+      <c r="S35" s="68">
         <f t="shared" si="6"/>
         <v>0.23189663375316114</v>
       </c>
-      <c r="T35" s="70">
+      <c r="T35" s="69">
         <f t="shared" si="6"/>
         <v>0.18492449633716196</v>
       </c>
+      <c r="U35" s="77"/>
       <c r="V35" s="5">
         <f t="shared" ref="V35" si="7">V21/V17</f>
         <v>0.31464139847030592</v>
       </c>
     </row>
-    <row r="36" spans="9:22" ht="15" thickBot="1">
-      <c r="I36" s="71" t="s">
+    <row r="36" spans="9:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="73">
+      <c r="J36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="72">
         <f>N7/N26</f>
         <v>19.290080428954425</v>
       </c>
-      <c r="O36" s="73">
+      <c r="O36" s="72">
         <f t="shared" ref="O36:V36" si="8">O7/O26</f>
         <v>17.181609195402299</v>
       </c>
-      <c r="P36" s="73">
+      <c r="P36" s="72">
         <f t="shared" si="8"/>
         <v>23.085173501577291</v>
       </c>
-      <c r="Q36" s="73">
+      <c r="Q36" s="72">
         <f t="shared" si="8"/>
         <v>19.946666666666665</v>
       </c>
-      <c r="R36" s="73">
+      <c r="R36" s="72">
         <f t="shared" si="8"/>
         <v>22.99334510389787</v>
       </c>
-      <c r="S36" s="73">
+      <c r="S36" s="72">
         <f t="shared" si="8"/>
         <v>17.654457788026715</v>
       </c>
-      <c r="T36" s="74">
+      <c r="T36" s="73">
         <f t="shared" si="8"/>
         <v>19.515929972116837</v>
       </c>
       <c r="U36" s="1"/>
-      <c r="V36" s="61">
+      <c r="V36" s="60">
         <f t="shared" si="8"/>
         <v>22.805288461538463</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>